<commit_message>
#78 adding changes for uploading match schedule in proper format
</commit_message>
<xml_diff>
--- a/src/main/data/match_schedule.xlsx
+++ b/src/main/data/match_schedule.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8F6145A-AC2A-B249-9C85-5124FC173C6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15C7050-090E-ED44-B79B-5424C7C8FDF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BE5D1743-4BEB-BD4C-825B-96829D86A2AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" xr2:uid="{BE5D1743-4BEB-BD4C-825B-96829D86A2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Home_Team</t>
   </si>
@@ -42,46 +43,43 @@
     <t>matchTime</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Mumbai Indians</t>
   </si>
   <si>
-    <t>Royal Chalenger</t>
-  </si>
-  <si>
     <t>IPL-20</t>
   </si>
   <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
     <t>2020-08-27T10:47:20.868Z</t>
   </si>
   <si>
-    <t>MI VS RCB - 08-27</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Delhi Capital</t>
-  </si>
-  <si>
-    <t>Kolkata knight riders</t>
-  </si>
-  <si>
-    <t>Chennai super kings</t>
-  </si>
-  <si>
-    <t>2020-09-27T10:47:20.868Z</t>
-  </si>
-  <si>
-    <t>2020-10-27T10:47:20.868Z</t>
+    <t>Royal Challengers Bengaluru</t>
+  </si>
+  <si>
+    <t>Chennai Super Kings</t>
+  </si>
+  <si>
+    <t>Sun Risers Hyderabad</t>
+  </si>
+  <si>
+    <t>2020-09-02T10:47:20.868Z</t>
+  </si>
+  <si>
+    <t>2020-09-05T10:47:20.868Z</t>
+  </si>
+  <si>
+    <t>2020-08-25T10:47:20.868Z</t>
+  </si>
+  <si>
+    <t>M. A. Chidambaram Stadium</t>
+  </si>
+  <si>
+    <t>Wankhede Stadium</t>
+  </si>
+  <si>
+    <t>Feroz Shah Kotla</t>
+  </si>
+  <si>
+    <t>Chinnaswamy Stadium</t>
   </si>
 </sst>
 </file>
@@ -433,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19900B3-89C6-4643-B4D8-14779E85D3BD}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,7 +446,97 @@
     <col min="6" max="6" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419ABE73-7812-0746-8EFA-2015A99B42F7}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="42.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,68 +552,73 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#167 adding changes for ui and some small fixes
</commit_message>
<xml_diff>
--- a/src/main/data/match_schedule.xlsx
+++ b/src/main/data/match_schedule.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D3A09C-6AD8-0442-A04C-3BD8DE6E476C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A97B56-F6E7-424D-AFEA-73E9D6A93041}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="140" windowWidth="40000" windowHeight="16220" xr2:uid="{BE5D1743-4BEB-BD4C-825B-96829D86A2AA}"/>
+    <workbookView xWindow="14160" yWindow="0" windowWidth="40000" windowHeight="16220" xr2:uid="{BE5D1743-4BEB-BD4C-825B-96829D86A2AA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Ipl Final Schedule" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="82">
   <si>
     <t>Home_Team</t>
   </si>
@@ -99,6 +100,180 @@
   </si>
   <si>
     <t>2020-09-19T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>SHARJAH</t>
+  </si>
+  <si>
+    <t>Sunrisers Hyderabad</t>
+  </si>
+  <si>
+    <t>Rajasthan Royals</t>
+  </si>
+  <si>
+    <t>Kolkata Knight Riders</t>
+  </si>
+  <si>
+    <t>2020-09-21T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-22T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-23T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-24T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-25T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-26T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-27T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-28T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-29T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-09-30T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-01T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-02T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-03T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-03T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-04T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-04T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-05T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-06T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-07T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-08T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-09T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-10T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-10T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-11T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-11T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-12T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-13T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-14T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-15T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-16T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-17T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-17T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-18T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-18T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-19T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-20T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-21T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-22T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-23T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-24T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-24T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-25T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-25T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-26T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-27T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-28T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-29T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-30T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-31T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-10-31T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-11-01T10:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-11-01T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-11-02T13:30:00.000Z</t>
+  </si>
+  <si>
+    <t>2020-11-03T13:30:00.000Z</t>
   </si>
 </sst>
 </file>
@@ -449,11 +624,966 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111EDD49-A26C-654B-9E35-B8C7C93DF47A}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A081745C-12F6-E646-9879-B3A05C9EA99E}">
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111EDD49-A26C-654B-9E35-B8C7C93DF47A}">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,12 +1645,930 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19900B3-89C6-4643-B4D8-14779E85D3BD}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -610,7 +2658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419ABE73-7812-0746-8EFA-2015A99B42F7}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>